<commit_message>
v 1.0.4 bug fixes
</commit_message>
<xml_diff>
--- a/SalesUtil/input - Copy.xlsx
+++ b/SalesUtil/input - Copy.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Visual Studio 2017\Projects\SalesUtil\SalesUtil\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\visual studio 2017\Projects\SalesUtil\SalesUtil\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21756" windowHeight="8964"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21756" windowHeight="8964"/>
   </bookViews>
   <sheets>
     <sheet name="Open" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
   </externalReferences>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -1884,7 +1884,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1925,13 +1925,9 @@
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2352,8 +2348,8 @@
   <sheetPr codeName="dataSheet"/>
   <dimension ref="A1:AC74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AB29" sqref="AB29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2461,7 +2457,7 @@
       <c r="X1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="39" t="s">
+      <c r="Y1" s="38" t="s">
         <v>24</v>
       </c>
       <c r="Z1" t="s">
@@ -2499,7 +2495,7 @@
       <c r="G2" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="H2" s="36" t="s">
+      <c r="H2" s="28" t="s">
         <v>275</v>
       </c>
       <c r="I2" s="9" t="s">
@@ -2553,7 +2549,7 @@
       <c r="Y2" s="25">
         <v>3</v>
       </c>
-      <c r="Z2" s="26">
+      <c r="Z2" s="29">
         <v>42972</v>
       </c>
       <c r="AA2" s="27" t="s">
@@ -2578,7 +2574,7 @@
       <c r="C3" s="3">
         <v>42915.784004629597</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="38" t="s">
         <v>263</v>
       </c>
       <c r="E3" s="5" t="s">
@@ -2644,7 +2640,7 @@
       <c r="Y3" s="25">
         <v>30</v>
       </c>
-      <c r="Z3" s="26">
+      <c r="Z3" s="29">
         <v>42977</v>
       </c>
       <c r="AA3" s="27" t="s">
@@ -2735,7 +2731,7 @@
       <c r="Y4" s="25">
         <v>42</v>
       </c>
-      <c r="Z4" s="26">
+      <c r="Z4" s="29">
         <v>42979</v>
       </c>
       <c r="AA4" s="27" t="s">
@@ -2760,7 +2756,7 @@
       <c r="C5" s="3">
         <v>42926.688923611102</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="D5" s="38" t="s">
         <v>191</v>
       </c>
       <c r="E5" s="5" t="s">
@@ -2954,7 +2950,7 @@
       <c r="G7" s="7" t="s">
         <v>332</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="28" t="s">
         <v>588</v>
       </c>
       <c r="I7" s="9" t="s">
@@ -3372,7 +3368,7 @@
       <c r="Y11" s="25">
         <v>48</v>
       </c>
-      <c r="Z11" s="26">
+      <c r="Z11" s="29">
         <v>42978</v>
       </c>
       <c r="AA11" s="31" t="s">
@@ -3400,7 +3396,7 @@
       <c r="G12" s="7" t="s">
         <v>572</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="28" t="s">
         <v>573</v>
       </c>
       <c r="I12" s="9" t="s">
@@ -3466,7 +3462,7 @@
       <c r="G13" s="7" t="s">
         <v>572</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="28" t="s">
         <v>577</v>
       </c>
       <c r="I13" s="9" t="s">
@@ -3532,7 +3528,7 @@
       <c r="G14" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="28" t="s">
         <v>580</v>
       </c>
       <c r="I14" s="9" t="s">
@@ -3607,7 +3603,7 @@
       <c r="G15" s="7" t="s">
         <v>341</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="H15" s="28" t="s">
         <v>342</v>
       </c>
       <c r="I15" s="9" t="s">
@@ -3689,7 +3685,7 @@
       <c r="G16" s="7" t="s">
         <v>557</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="H16" s="28" t="s">
         <v>558</v>
       </c>
       <c r="I16" s="9" t="s">
@@ -3824,7 +3820,7 @@
       <c r="E18" s="5" t="s">
         <v>524</v>
       </c>
-      <c r="F18" s="37" t="s">
+      <c r="F18" s="36" t="s">
         <v>525</v>
       </c>
       <c r="G18" s="7" t="s">
@@ -4467,7 +4463,7 @@
       <c r="G25" s="7" t="s">
         <v>405</v>
       </c>
-      <c r="H25" s="8" t="s">
+      <c r="H25" s="28" t="s">
         <v>406</v>
       </c>
       <c r="I25" s="9" t="s">
@@ -4791,7 +4787,7 @@
       <c r="X28" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="Y28" s="40">
+      <c r="Y28" s="30">
         <v>1</v>
       </c>
       <c r="Z28" s="29">
@@ -4831,7 +4827,7 @@
       <c r="G29" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="H29" s="8" t="s">
+      <c r="H29" s="28" t="s">
         <v>53</v>
       </c>
       <c r="I29" s="9" t="s">
@@ -4922,7 +4918,7 @@
       <c r="G30" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H30" s="8" t="s">
+      <c r="H30" s="28" t="s">
         <v>33</v>
       </c>
       <c r="I30" s="9" t="s">
@@ -5013,7 +5009,7 @@
       <c r="G31" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H31" s="8" t="s">
+      <c r="H31" s="28" t="s">
         <v>33</v>
       </c>
       <c r="I31" s="9" t="s">
@@ -5104,7 +5100,7 @@
       <c r="G32" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="H32" s="8" t="s">
+      <c r="H32" s="28" t="s">
         <v>53</v>
       </c>
       <c r="I32" s="9" t="s">
@@ -5158,7 +5154,7 @@
       <c r="Y32" s="25">
         <v>2</v>
       </c>
-      <c r="Z32" s="26">
+      <c r="Z32" s="29">
         <v>42972</v>
       </c>
       <c r="AA32" s="31" t="s">
@@ -5377,7 +5373,7 @@
       <c r="G35" s="7" t="s">
         <v>499</v>
       </c>
-      <c r="H35" s="8" t="s">
+      <c r="H35" s="28" t="s">
         <v>500</v>
       </c>
       <c r="I35" s="9" t="s">
@@ -5468,7 +5464,7 @@
       <c r="G36" s="7" t="s">
         <v>396</v>
       </c>
-      <c r="H36" s="8" t="s">
+      <c r="H36" s="28" t="s">
         <v>397</v>
       </c>
       <c r="I36" s="9" t="s">
@@ -5559,7 +5555,7 @@
       <c r="G37" s="7" t="s">
         <v>452</v>
       </c>
-      <c r="H37" s="8" t="s">
+      <c r="H37" s="28" t="s">
         <v>397</v>
       </c>
       <c r="I37" s="9" t="s">
@@ -5650,7 +5646,7 @@
       <c r="G38" s="7" t="s">
         <v>452</v>
       </c>
-      <c r="H38" s="8" t="s">
+      <c r="H38" s="28" t="s">
         <v>397</v>
       </c>
       <c r="I38" s="9" t="s">
@@ -5832,7 +5828,7 @@
       <c r="G40" s="7" t="s">
         <v>439</v>
       </c>
-      <c r="H40" s="8" t="s">
+      <c r="H40" s="28" t="s">
         <v>53</v>
       </c>
       <c r="I40" s="9" t="s">
@@ -6469,7 +6465,7 @@
       <c r="G47" s="7" t="s">
         <v>416</v>
       </c>
-      <c r="H47" s="8" t="s">
+      <c r="H47" s="28" t="s">
         <v>53</v>
       </c>
       <c r="I47" s="9" t="s">
@@ -6796,7 +6792,7 @@
       <c r="Y50" s="30">
         <v>1</v>
       </c>
-      <c r="Z50" s="26">
+      <c r="Z50" s="29">
         <v>42967</v>
       </c>
       <c r="AA50" s="27" t="s">
@@ -6887,7 +6883,7 @@
       <c r="Y51" s="30">
         <v>1</v>
       </c>
-      <c r="Z51" s="26">
+      <c r="Z51" s="29">
         <v>42978</v>
       </c>
       <c r="AA51" s="27" t="s">
@@ -6978,7 +6974,7 @@
       <c r="Y52" s="25">
         <v>6</v>
       </c>
-      <c r="Z52" s="26">
+      <c r="Z52" s="29">
         <v>42979</v>
       </c>
       <c r="AA52" s="27" t="s">
@@ -7257,7 +7253,7 @@
       <c r="E56" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F56" s="38" t="s">
+      <c r="F56" s="37" t="s">
         <v>152</v>
       </c>
       <c r="G56" s="7" t="s">
@@ -8355,7 +8351,7 @@
       <c r="G68" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="H68" s="8" t="s">
+      <c r="H68" s="28" t="s">
         <v>53</v>
       </c>
       <c r="I68" s="9" t="s">
@@ -8446,7 +8442,7 @@
       <c r="G69" s="27" t="s">
         <v>216</v>
       </c>
-      <c r="H69" s="8" t="s">
+      <c r="H69" s="28" t="s">
         <v>53</v>
       </c>
       <c r="I69" s="27" t="s">
@@ -8500,7 +8496,7 @@
       <c r="Y69" s="25">
         <v>6</v>
       </c>
-      <c r="Z69" s="26">
+      <c r="Z69" s="29">
         <v>42981</v>
       </c>
       <c r="AA69" s="27" t="s">
@@ -8537,7 +8533,7 @@
       <c r="G70" s="27" t="s">
         <v>352</v>
       </c>
-      <c r="H70" s="8" t="s">
+      <c r="H70" s="28" t="s">
         <v>375</v>
       </c>
       <c r="I70" s="27" t="s">
@@ -8628,7 +8624,7 @@
       <c r="G71" s="27" t="s">
         <v>352</v>
       </c>
-      <c r="H71" s="8" t="s">
+      <c r="H71" s="28" t="s">
         <v>353</v>
       </c>
       <c r="I71" s="27" t="s">
@@ -8719,7 +8715,7 @@
       <c r="G72" s="27" t="s">
         <v>444</v>
       </c>
-      <c r="H72" s="8" t="s">
+      <c r="H72" s="28" t="s">
         <v>53</v>
       </c>
       <c r="I72" s="27" t="s">
@@ -8810,7 +8806,7 @@
       <c r="G73" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="H73" s="8" t="s">
+      <c r="H73" s="28" t="s">
         <v>52</v>
       </c>
       <c r="I73" s="27" t="s">
@@ -8901,7 +8897,7 @@
       <c r="G74" s="27" t="s">
         <v>370</v>
       </c>
-      <c r="H74" s="8" t="s">
+      <c r="H74" s="28" t="s">
         <v>53</v>
       </c>
       <c r="I74" s="27" t="s">

</xml_diff>